<commit_message>
Add cleaned elasticity, price, and quantity data
- Updated data collection functions
- Minor fixes to original data
</commit_message>
<xml_diff>
--- a/data/Elasticity_Data.xlsx
+++ b/data/Elasticity_Data.xlsx
@@ -1325,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC523"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A433" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G444" sqref="G444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1336,7 @@
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
     <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -31691,7 +31691,7 @@
         <v>262</v>
       </c>
       <c r="G443">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="H443" t="s">
         <v>274</v>

</xml_diff>